<commit_message>
Add/Update Quantities.xlsx via API
</commit_message>
<xml_diff>
--- a/Quantities.xlsx
+++ b/Quantities.xlsx
@@ -58,7 +58,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -66,7 +66,6 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -432,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K178"/>
+  <dimension ref="A1:J177"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,15 +485,10 @@
           <t>TRXUSDT</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>index</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>25569</v>
+        <v>45558</v>
       </c>
       <c r="B2" t="n">
         <v>116.4121952</v>
@@ -523,13 +517,10 @@
       <c r="J2" t="n">
         <v>1941.48834923</v>
       </c>
-      <c r="K2" s="3" t="n">
-        <v>45558</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45558</v>
+        <v>45559</v>
       </c>
       <c r="B3" t="n">
         <v>116.4121952</v>
@@ -558,17 +549,16 @@
       <c r="J3" t="n">
         <v>1941.48834923</v>
       </c>
-      <c r="K3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45559</v>
+        <v>45560</v>
       </c>
       <c r="B4" t="n">
         <v>116.4121952</v>
       </c>
       <c r="C4" t="n">
-        <v>4.012e-05</v>
+        <v>0.00170247</v>
       </c>
       <c r="D4" t="n">
         <v>0.008850780000000001</v>
@@ -580,7 +570,7 @@
         <v>12792.90181321</v>
       </c>
       <c r="G4" t="n">
-        <v>280.99031254</v>
+        <v>465.80531254</v>
       </c>
       <c r="H4" t="n">
         <v>0.24</v>
@@ -589,13 +579,12 @@
         <v>1.7904431</v>
       </c>
       <c r="J4" t="n">
-        <v>1941.48834923</v>
-      </c>
-      <c r="K4" t="inlineStr"/>
+        <v>485.38834923</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45560</v>
+        <v>45561</v>
       </c>
       <c r="B5" t="n">
         <v>116.4121952</v>
@@ -624,11 +613,10 @@
       <c r="J5" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45561</v>
+        <v>45562</v>
       </c>
       <c r="B6" t="n">
         <v>116.4121952</v>
@@ -657,11 +645,10 @@
       <c r="J6" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45562</v>
+        <v>45563</v>
       </c>
       <c r="B7" t="n">
         <v>116.4121952</v>
@@ -690,11 +677,10 @@
       <c r="J7" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45563</v>
+        <v>45564</v>
       </c>
       <c r="B8" t="n">
         <v>116.4121952</v>
@@ -723,11 +709,10 @@
       <c r="J8" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45564</v>
+        <v>45565</v>
       </c>
       <c r="B9" t="n">
         <v>116.4121952</v>
@@ -756,11 +741,10 @@
       <c r="J9" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45565</v>
+        <v>45566</v>
       </c>
       <c r="B10" t="n">
         <v>116.4121952</v>
@@ -789,11 +773,10 @@
       <c r="J10" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45566</v>
+        <v>45567</v>
       </c>
       <c r="B11" t="n">
         <v>116.4121952</v>
@@ -822,11 +805,10 @@
       <c r="J11" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45567</v>
+        <v>45568</v>
       </c>
       <c r="B12" t="n">
         <v>116.4121952</v>
@@ -855,11 +837,10 @@
       <c r="J12" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45568</v>
+        <v>45569</v>
       </c>
       <c r="B13" t="n">
         <v>116.4121952</v>
@@ -888,11 +869,10 @@
       <c r="J13" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45569</v>
+        <v>45570</v>
       </c>
       <c r="B14" t="n">
         <v>116.4121952</v>
@@ -921,11 +901,10 @@
       <c r="J14" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45570</v>
+        <v>45571</v>
       </c>
       <c r="B15" t="n">
         <v>116.4121952</v>
@@ -954,11 +933,10 @@
       <c r="J15" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>45571</v>
+        <v>45572</v>
       </c>
       <c r="B16" t="n">
         <v>116.4121952</v>
@@ -987,11 +965,10 @@
       <c r="J16" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45572</v>
+        <v>45573</v>
       </c>
       <c r="B17" t="n">
         <v>116.4121952</v>
@@ -1020,11 +997,10 @@
       <c r="J17" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45573</v>
+        <v>45574</v>
       </c>
       <c r="B18" t="n">
         <v>116.4121952</v>
@@ -1053,11 +1029,10 @@
       <c r="J18" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>45574</v>
+        <v>45575</v>
       </c>
       <c r="B19" t="n">
         <v>116.4121952</v>
@@ -1086,11 +1061,10 @@
       <c r="J19" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>45575</v>
+        <v>45576</v>
       </c>
       <c r="B20" t="n">
         <v>116.4121952</v>
@@ -1119,11 +1093,10 @@
       <c r="J20" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>45576</v>
+        <v>45577</v>
       </c>
       <c r="B21" t="n">
         <v>116.4121952</v>
@@ -1152,11 +1125,10 @@
       <c r="J21" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>45577</v>
+        <v>45578</v>
       </c>
       <c r="B22" t="n">
         <v>116.4121952</v>
@@ -1185,11 +1157,10 @@
       <c r="J22" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>45578</v>
+        <v>45579</v>
       </c>
       <c r="B23" t="n">
         <v>116.4121952</v>
@@ -1218,11 +1189,10 @@
       <c r="J23" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>45579</v>
+        <v>45580</v>
       </c>
       <c r="B24" t="n">
         <v>116.4121952</v>
@@ -1251,11 +1221,10 @@
       <c r="J24" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>45580</v>
+        <v>45581</v>
       </c>
       <c r="B25" t="n">
         <v>116.4121952</v>
@@ -1284,11 +1253,10 @@
       <c r="J25" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>45581</v>
+        <v>45582</v>
       </c>
       <c r="B26" t="n">
         <v>116.4121952</v>
@@ -1317,11 +1285,10 @@
       <c r="J26" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>45582</v>
+        <v>45583</v>
       </c>
       <c r="B27" t="n">
         <v>116.4121952</v>
@@ -1350,11 +1317,10 @@
       <c r="J27" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>45583</v>
+        <v>45584</v>
       </c>
       <c r="B28" t="n">
         <v>116.4121952</v>
@@ -1383,11 +1349,10 @@
       <c r="J28" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>45584</v>
+        <v>45585</v>
       </c>
       <c r="B29" t="n">
         <v>116.4121952</v>
@@ -1416,11 +1381,10 @@
       <c r="J29" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>45585</v>
+        <v>45586</v>
       </c>
       <c r="B30" t="n">
         <v>116.4121952</v>
@@ -1449,11 +1413,10 @@
       <c r="J30" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>45586</v>
+        <v>45587</v>
       </c>
       <c r="B31" t="n">
         <v>116.4121952</v>
@@ -1482,11 +1445,10 @@
       <c r="J31" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>45587</v>
+        <v>45588</v>
       </c>
       <c r="B32" t="n">
         <v>116.4121952</v>
@@ -1515,11 +1477,10 @@
       <c r="J32" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>45588</v>
+        <v>45589</v>
       </c>
       <c r="B33" t="n">
         <v>116.4121952</v>
@@ -1548,11 +1509,10 @@
       <c r="J33" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>45589</v>
+        <v>45590</v>
       </c>
       <c r="B34" t="n">
         <v>116.4121952</v>
@@ -1581,11 +1541,10 @@
       <c r="J34" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>45590</v>
+        <v>45591</v>
       </c>
       <c r="B35" t="n">
         <v>116.4121952</v>
@@ -1614,11 +1573,10 @@
       <c r="J35" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>45591</v>
+        <v>45592</v>
       </c>
       <c r="B36" t="n">
         <v>116.4121952</v>
@@ -1647,11 +1605,10 @@
       <c r="J36" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>45592</v>
+        <v>45593</v>
       </c>
       <c r="B37" t="n">
         <v>116.4121952</v>
@@ -1680,11 +1637,10 @@
       <c r="J37" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>45593</v>
+        <v>45594</v>
       </c>
       <c r="B38" t="n">
         <v>116.4121952</v>
@@ -1713,11 +1669,10 @@
       <c r="J38" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>45594</v>
+        <v>45595</v>
       </c>
       <c r="B39" t="n">
         <v>116.4121952</v>
@@ -1746,11 +1701,10 @@
       <c r="J39" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>45595</v>
+        <v>45596</v>
       </c>
       <c r="B40" t="n">
         <v>116.4121952</v>
@@ -1779,11 +1733,10 @@
       <c r="J40" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>45596</v>
+        <v>45597</v>
       </c>
       <c r="B41" t="n">
         <v>116.4121952</v>
@@ -1812,11 +1765,10 @@
       <c r="J41" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>45597</v>
+        <v>45598</v>
       </c>
       <c r="B42" t="n">
         <v>116.4121952</v>
@@ -1845,11 +1797,10 @@
       <c r="J42" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>45598</v>
+        <v>45599</v>
       </c>
       <c r="B43" t="n">
         <v>116.4121952</v>
@@ -1878,11 +1829,10 @@
       <c r="J43" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
-        <v>45599</v>
+        <v>45600</v>
       </c>
       <c r="B44" t="n">
         <v>116.4121952</v>
@@ -1911,11 +1861,10 @@
       <c r="J44" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
-        <v>45600</v>
+        <v>45601</v>
       </c>
       <c r="B45" t="n">
         <v>116.4121952</v>
@@ -1944,11 +1893,10 @@
       <c r="J45" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
-        <v>45601</v>
+        <v>45602</v>
       </c>
       <c r="B46" t="n">
         <v>116.4121952</v>
@@ -1977,11 +1925,10 @@
       <c r="J46" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
-        <v>45602</v>
+        <v>45603</v>
       </c>
       <c r="B47" t="n">
         <v>116.4121952</v>
@@ -2010,11 +1957,10 @@
       <c r="J47" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
-        <v>45603</v>
+        <v>45604</v>
       </c>
       <c r="B48" t="n">
         <v>116.4121952</v>
@@ -2043,11 +1989,10 @@
       <c r="J48" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
-        <v>45604</v>
+        <v>45605</v>
       </c>
       <c r="B49" t="n">
         <v>116.4121952</v>
@@ -2076,11 +2021,10 @@
       <c r="J49" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" s="2" t="n">
-        <v>45605</v>
+        <v>45606</v>
       </c>
       <c r="B50" t="n">
         <v>116.4121952</v>
@@ -2109,11 +2053,10 @@
       <c r="J50" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" s="2" t="n">
-        <v>45606</v>
+        <v>45607</v>
       </c>
       <c r="B51" t="n">
         <v>116.4121952</v>
@@ -2142,11 +2085,10 @@
       <c r="J51" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" s="2" t="n">
-        <v>45607</v>
+        <v>45608</v>
       </c>
       <c r="B52" t="n">
         <v>116.4121952</v>
@@ -2175,11 +2117,10 @@
       <c r="J52" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" s="2" t="n">
-        <v>45608</v>
+        <v>45609</v>
       </c>
       <c r="B53" t="n">
         <v>116.4121952</v>
@@ -2208,11 +2149,10 @@
       <c r="J53" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" s="2" t="n">
-        <v>45609</v>
+        <v>45610</v>
       </c>
       <c r="B54" t="n">
         <v>116.4121952</v>
@@ -2241,11 +2181,10 @@
       <c r="J54" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" s="2" t="n">
-        <v>45610</v>
+        <v>45611</v>
       </c>
       <c r="B55" t="n">
         <v>116.4121952</v>
@@ -2274,11 +2213,10 @@
       <c r="J55" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" s="2" t="n">
-        <v>45611</v>
+        <v>45612</v>
       </c>
       <c r="B56" t="n">
         <v>116.4121952</v>
@@ -2307,11 +2245,10 @@
       <c r="J56" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" s="2" t="n">
-        <v>45612</v>
+        <v>45613</v>
       </c>
       <c r="B57" t="n">
         <v>116.4121952</v>
@@ -2340,11 +2277,10 @@
       <c r="J57" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" s="2" t="n">
-        <v>45613</v>
+        <v>45614</v>
       </c>
       <c r="B58" t="n">
         <v>116.4121952</v>
@@ -2373,11 +2309,10 @@
       <c r="J58" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" s="2" t="n">
-        <v>45614</v>
+        <v>45615</v>
       </c>
       <c r="B59" t="n">
         <v>116.4121952</v>
@@ -2406,11 +2341,10 @@
       <c r="J59" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" s="2" t="n">
-        <v>45615</v>
+        <v>45616</v>
       </c>
       <c r="B60" t="n">
         <v>116.4121952</v>
@@ -2439,11 +2373,10 @@
       <c r="J60" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" s="2" t="n">
-        <v>45616</v>
+        <v>45617</v>
       </c>
       <c r="B61" t="n">
         <v>116.4121952</v>
@@ -2472,11 +2405,10 @@
       <c r="J61" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" s="2" t="n">
-        <v>45617</v>
+        <v>45618</v>
       </c>
       <c r="B62" t="n">
         <v>116.4121952</v>
@@ -2505,11 +2437,10 @@
       <c r="J62" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" s="2" t="n">
-        <v>45618</v>
+        <v>45619</v>
       </c>
       <c r="B63" t="n">
         <v>116.4121952</v>
@@ -2538,11 +2469,10 @@
       <c r="J63" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" s="2" t="n">
-        <v>45619</v>
+        <v>45620</v>
       </c>
       <c r="B64" t="n">
         <v>116.4121952</v>
@@ -2571,11 +2501,10 @@
       <c r="J64" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" s="2" t="n">
-        <v>45620</v>
+        <v>45621</v>
       </c>
       <c r="B65" t="n">
         <v>116.4121952</v>
@@ -2604,11 +2533,10 @@
       <c r="J65" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" s="2" t="n">
-        <v>45621</v>
+        <v>45622</v>
       </c>
       <c r="B66" t="n">
         <v>116.4121952</v>
@@ -2637,11 +2565,10 @@
       <c r="J66" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" s="2" t="n">
-        <v>45622</v>
+        <v>45623</v>
       </c>
       <c r="B67" t="n">
         <v>116.4121952</v>
@@ -2670,11 +2597,10 @@
       <c r="J67" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" s="2" t="n">
-        <v>45623</v>
+        <v>45624</v>
       </c>
       <c r="B68" t="n">
         <v>116.4121952</v>
@@ -2703,11 +2629,10 @@
       <c r="J68" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" s="2" t="n">
-        <v>45624</v>
+        <v>45625</v>
       </c>
       <c r="B69" t="n">
         <v>116.4121952</v>
@@ -2736,11 +2661,10 @@
       <c r="J69" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" s="2" t="n">
-        <v>45625</v>
+        <v>45626</v>
       </c>
       <c r="B70" t="n">
         <v>116.4121952</v>
@@ -2769,11 +2693,10 @@
       <c r="J70" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" s="2" t="n">
-        <v>45626</v>
+        <v>45627</v>
       </c>
       <c r="B71" t="n">
         <v>116.4121952</v>
@@ -2802,11 +2725,10 @@
       <c r="J71" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" s="2" t="n">
-        <v>45627</v>
+        <v>45628</v>
       </c>
       <c r="B72" t="n">
         <v>116.4121952</v>
@@ -2835,11 +2757,10 @@
       <c r="J72" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" s="2" t="n">
-        <v>45628</v>
+        <v>45629</v>
       </c>
       <c r="B73" t="n">
         <v>116.4121952</v>
@@ -2868,11 +2789,10 @@
       <c r="J73" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" s="2" t="n">
-        <v>45629</v>
+        <v>45630</v>
       </c>
       <c r="B74" t="n">
         <v>116.4121952</v>
@@ -2901,11 +2821,10 @@
       <c r="J74" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" s="2" t="n">
-        <v>45630</v>
+        <v>45631</v>
       </c>
       <c r="B75" t="n">
         <v>116.4121952</v>
@@ -2934,11 +2853,10 @@
       <c r="J75" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" s="2" t="n">
-        <v>45631</v>
+        <v>45632</v>
       </c>
       <c r="B76" t="n">
         <v>116.4121952</v>
@@ -2967,11 +2885,10 @@
       <c r="J76" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" s="2" t="n">
-        <v>45632</v>
+        <v>45633</v>
       </c>
       <c r="B77" t="n">
         <v>116.4121952</v>
@@ -3000,11 +2917,10 @@
       <c r="J77" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" s="2" t="n">
-        <v>45633</v>
+        <v>45634</v>
       </c>
       <c r="B78" t="n">
         <v>116.4121952</v>
@@ -3033,11 +2949,10 @@
       <c r="J78" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" s="2" t="n">
-        <v>45634</v>
+        <v>45635</v>
       </c>
       <c r="B79" t="n">
         <v>116.4121952</v>
@@ -3066,11 +2981,10 @@
       <c r="J79" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" s="2" t="n">
-        <v>45635</v>
+        <v>45636</v>
       </c>
       <c r="B80" t="n">
         <v>116.4121952</v>
@@ -3099,11 +3013,10 @@
       <c r="J80" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" s="2" t="n">
-        <v>45636</v>
+        <v>45637</v>
       </c>
       <c r="B81" t="n">
         <v>116.4121952</v>
@@ -3132,11 +3045,10 @@
       <c r="J81" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" s="2" t="n">
-        <v>45637</v>
+        <v>45638</v>
       </c>
       <c r="B82" t="n">
         <v>116.4121952</v>
@@ -3165,11 +3077,10 @@
       <c r="J82" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" s="2" t="n">
-        <v>45638</v>
+        <v>45639</v>
       </c>
       <c r="B83" t="n">
         <v>116.4121952</v>
@@ -3198,11 +3109,10 @@
       <c r="J83" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" s="2" t="n">
-        <v>45639</v>
+        <v>45640</v>
       </c>
       <c r="B84" t="n">
         <v>116.4121952</v>
@@ -3231,11 +3141,10 @@
       <c r="J84" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" s="2" t="n">
-        <v>45640</v>
+        <v>45641</v>
       </c>
       <c r="B85" t="n">
         <v>116.4121952</v>
@@ -3264,11 +3173,10 @@
       <c r="J85" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" s="2" t="n">
-        <v>45641</v>
+        <v>45642</v>
       </c>
       <c r="B86" t="n">
         <v>116.4121952</v>
@@ -3297,11 +3205,10 @@
       <c r="J86" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" s="2" t="n">
-        <v>45642</v>
+        <v>45643</v>
       </c>
       <c r="B87" t="n">
         <v>116.4121952</v>
@@ -3330,11 +3237,10 @@
       <c r="J87" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" s="2" t="n">
-        <v>45643</v>
+        <v>45644</v>
       </c>
       <c r="B88" t="n">
         <v>116.4121952</v>
@@ -3363,11 +3269,10 @@
       <c r="J88" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" s="2" t="n">
-        <v>45644</v>
+        <v>45645</v>
       </c>
       <c r="B89" t="n">
         <v>116.4121952</v>
@@ -3396,11 +3301,10 @@
       <c r="J89" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" s="2" t="n">
-        <v>45645</v>
+        <v>45646</v>
       </c>
       <c r="B90" t="n">
         <v>116.4121952</v>
@@ -3429,11 +3333,10 @@
       <c r="J90" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" s="2" t="n">
-        <v>45646</v>
+        <v>45647</v>
       </c>
       <c r="B91" t="n">
         <v>116.4121952</v>
@@ -3462,11 +3365,10 @@
       <c r="J91" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" s="2" t="n">
-        <v>45647</v>
+        <v>45648</v>
       </c>
       <c r="B92" t="n">
         <v>116.4121952</v>
@@ -3495,11 +3397,10 @@
       <c r="J92" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" s="2" t="n">
-        <v>45648</v>
+        <v>45649</v>
       </c>
       <c r="B93" t="n">
         <v>116.4121952</v>
@@ -3528,11 +3429,10 @@
       <c r="J93" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" s="2" t="n">
-        <v>45649</v>
+        <v>45650</v>
       </c>
       <c r="B94" t="n">
         <v>116.4121952</v>
@@ -3561,11 +3461,10 @@
       <c r="J94" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" s="2" t="n">
-        <v>45650</v>
+        <v>45651</v>
       </c>
       <c r="B95" t="n">
         <v>116.4121952</v>
@@ -3594,11 +3493,10 @@
       <c r="J95" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" s="2" t="n">
-        <v>45651</v>
+        <v>45652</v>
       </c>
       <c r="B96" t="n">
         <v>116.4121952</v>
@@ -3627,11 +3525,10 @@
       <c r="J96" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" s="2" t="n">
-        <v>45652</v>
+        <v>45653</v>
       </c>
       <c r="B97" t="n">
         <v>116.4121952</v>
@@ -3660,11 +3557,10 @@
       <c r="J97" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" s="2" t="n">
-        <v>45653</v>
+        <v>45654</v>
       </c>
       <c r="B98" t="n">
         <v>116.4121952</v>
@@ -3693,11 +3589,10 @@
       <c r="J98" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" s="2" t="n">
-        <v>45654</v>
+        <v>45655</v>
       </c>
       <c r="B99" t="n">
         <v>116.4121952</v>
@@ -3726,11 +3621,10 @@
       <c r="J99" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" s="2" t="n">
-        <v>45655</v>
+        <v>45656</v>
       </c>
       <c r="B100" t="n">
         <v>116.4121952</v>
@@ -3759,11 +3653,10 @@
       <c r="J100" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" s="2" t="n">
-        <v>45656</v>
+        <v>45657</v>
       </c>
       <c r="B101" t="n">
         <v>116.4121952</v>
@@ -3792,11 +3685,10 @@
       <c r="J101" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" s="2" t="n">
-        <v>45657</v>
+        <v>45658</v>
       </c>
       <c r="B102" t="n">
         <v>116.4121952</v>
@@ -3825,11 +3717,10 @@
       <c r="J102" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" s="2" t="n">
-        <v>45658</v>
+        <v>45659</v>
       </c>
       <c r="B103" t="n">
         <v>116.4121952</v>
@@ -3858,11 +3749,10 @@
       <c r="J103" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" s="2" t="n">
-        <v>45659</v>
+        <v>45660</v>
       </c>
       <c r="B104" t="n">
         <v>116.4121952</v>
@@ -3891,11 +3781,10 @@
       <c r="J104" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" s="2" t="n">
-        <v>45660</v>
+        <v>45661</v>
       </c>
       <c r="B105" t="n">
         <v>116.4121952</v>
@@ -3924,11 +3813,10 @@
       <c r="J105" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" s="2" t="n">
-        <v>45661</v>
+        <v>45662</v>
       </c>
       <c r="B106" t="n">
         <v>116.4121952</v>
@@ -3957,11 +3845,10 @@
       <c r="J106" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" s="2" t="n">
-        <v>45662</v>
+        <v>45663</v>
       </c>
       <c r="B107" t="n">
         <v>116.4121952</v>
@@ -3990,11 +3877,10 @@
       <c r="J107" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" s="2" t="n">
-        <v>45663</v>
+        <v>45664</v>
       </c>
       <c r="B108" t="n">
         <v>116.4121952</v>
@@ -4023,11 +3909,10 @@
       <c r="J108" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" s="2" t="n">
-        <v>45664</v>
+        <v>45665</v>
       </c>
       <c r="B109" t="n">
         <v>116.4121952</v>
@@ -4056,11 +3941,10 @@
       <c r="J109" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" s="2" t="n">
-        <v>45665</v>
+        <v>45666</v>
       </c>
       <c r="B110" t="n">
         <v>116.4121952</v>
@@ -4089,11 +3973,10 @@
       <c r="J110" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" s="2" t="n">
-        <v>45666</v>
+        <v>45667</v>
       </c>
       <c r="B111" t="n">
         <v>116.4121952</v>
@@ -4122,11 +4005,10 @@
       <c r="J111" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" s="2" t="n">
-        <v>45667</v>
+        <v>45668</v>
       </c>
       <c r="B112" t="n">
         <v>116.4121952</v>
@@ -4155,11 +4037,10 @@
       <c r="J112" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" s="2" t="n">
-        <v>45668</v>
+        <v>45669</v>
       </c>
       <c r="B113" t="n">
         <v>116.4121952</v>
@@ -4188,11 +4069,10 @@
       <c r="J113" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" s="2" t="n">
-        <v>45669</v>
+        <v>45670</v>
       </c>
       <c r="B114" t="n">
         <v>116.4121952</v>
@@ -4221,11 +4101,10 @@
       <c r="J114" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" s="2" t="n">
-        <v>45670</v>
+        <v>45671</v>
       </c>
       <c r="B115" t="n">
         <v>116.4121952</v>
@@ -4254,11 +4133,10 @@
       <c r="J115" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" s="2" t="n">
-        <v>45671</v>
+        <v>45672</v>
       </c>
       <c r="B116" t="n">
         <v>116.4121952</v>
@@ -4287,11 +4165,10 @@
       <c r="J116" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" s="2" t="n">
-        <v>45672</v>
+        <v>45673</v>
       </c>
       <c r="B117" t="n">
         <v>116.4121952</v>
@@ -4320,11 +4197,10 @@
       <c r="J117" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" s="2" t="n">
-        <v>45673</v>
+        <v>45674</v>
       </c>
       <c r="B118" t="n">
         <v>116.4121952</v>
@@ -4353,11 +4229,10 @@
       <c r="J118" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" s="2" t="n">
-        <v>45674</v>
+        <v>45675</v>
       </c>
       <c r="B119" t="n">
         <v>116.4121952</v>
@@ -4386,11 +4261,10 @@
       <c r="J119" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" s="2" t="n">
-        <v>45675</v>
+        <v>45676</v>
       </c>
       <c r="B120" t="n">
         <v>116.4121952</v>
@@ -4419,11 +4293,10 @@
       <c r="J120" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" s="2" t="n">
-        <v>45676</v>
+        <v>45677</v>
       </c>
       <c r="B121" t="n">
         <v>116.4121952</v>
@@ -4452,11 +4325,10 @@
       <c r="J121" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" s="2" t="n">
-        <v>45677</v>
+        <v>45678</v>
       </c>
       <c r="B122" t="n">
         <v>116.4121952</v>
@@ -4485,11 +4357,10 @@
       <c r="J122" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K122" t="inlineStr"/>
     </row>
     <row r="123">
       <c r="A123" s="2" t="n">
-        <v>45678</v>
+        <v>45679</v>
       </c>
       <c r="B123" t="n">
         <v>116.4121952</v>
@@ -4518,11 +4389,10 @@
       <c r="J123" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" s="2" t="n">
-        <v>45679</v>
+        <v>45680</v>
       </c>
       <c r="B124" t="n">
         <v>116.4121952</v>
@@ -4551,11 +4421,10 @@
       <c r="J124" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" s="2" t="n">
-        <v>45680</v>
+        <v>45681</v>
       </c>
       <c r="B125" t="n">
         <v>116.4121952</v>
@@ -4584,11 +4453,10 @@
       <c r="J125" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K125" t="inlineStr"/>
     </row>
     <row r="126">
       <c r="A126" s="2" t="n">
-        <v>45681</v>
+        <v>45682</v>
       </c>
       <c r="B126" t="n">
         <v>116.4121952</v>
@@ -4617,11 +4485,10 @@
       <c r="J126" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" s="2" t="n">
-        <v>45682</v>
+        <v>45683</v>
       </c>
       <c r="B127" t="n">
         <v>116.4121952</v>
@@ -4650,11 +4517,10 @@
       <c r="J127" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" s="2" t="n">
-        <v>45683</v>
+        <v>45684</v>
       </c>
       <c r="B128" t="n">
         <v>116.4121952</v>
@@ -4683,11 +4549,10 @@
       <c r="J128" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" s="2" t="n">
-        <v>45684</v>
+        <v>45685</v>
       </c>
       <c r="B129" t="n">
         <v>116.4121952</v>
@@ -4716,11 +4581,10 @@
       <c r="J129" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" s="2" t="n">
-        <v>45685</v>
+        <v>45686</v>
       </c>
       <c r="B130" t="n">
         <v>116.4121952</v>
@@ -4749,11 +4613,10 @@
       <c r="J130" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" s="2" t="n">
-        <v>45686</v>
+        <v>45687</v>
       </c>
       <c r="B131" t="n">
         <v>116.4121952</v>
@@ -4782,11 +4645,10 @@
       <c r="J131" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" s="2" t="n">
-        <v>45687</v>
+        <v>45688</v>
       </c>
       <c r="B132" t="n">
         <v>116.4121952</v>
@@ -4815,11 +4677,10 @@
       <c r="J132" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" s="2" t="n">
-        <v>45688</v>
+        <v>45689</v>
       </c>
       <c r="B133" t="n">
         <v>116.4121952</v>
@@ -4848,11 +4709,10 @@
       <c r="J133" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" s="2" t="n">
-        <v>45689</v>
+        <v>45690</v>
       </c>
       <c r="B134" t="n">
         <v>116.4121952</v>
@@ -4881,11 +4741,10 @@
       <c r="J134" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" s="2" t="n">
-        <v>45690</v>
+        <v>45691</v>
       </c>
       <c r="B135" t="n">
         <v>116.4121952</v>
@@ -4914,11 +4773,10 @@
       <c r="J135" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" s="2" t="n">
-        <v>45691</v>
+        <v>45692</v>
       </c>
       <c r="B136" t="n">
         <v>116.4121952</v>
@@ -4947,11 +4805,10 @@
       <c r="J136" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" s="2" t="n">
-        <v>45692</v>
+        <v>45693</v>
       </c>
       <c r="B137" t="n">
         <v>116.4121952</v>
@@ -4980,11 +4837,10 @@
       <c r="J137" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" s="2" t="n">
-        <v>45693</v>
+        <v>45694</v>
       </c>
       <c r="B138" t="n">
         <v>116.4121952</v>
@@ -5013,11 +4869,10 @@
       <c r="J138" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" s="2" t="n">
-        <v>45694</v>
+        <v>45695</v>
       </c>
       <c r="B139" t="n">
         <v>116.4121952</v>
@@ -5046,11 +4901,10 @@
       <c r="J139" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" s="2" t="n">
-        <v>45695</v>
+        <v>45696</v>
       </c>
       <c r="B140" t="n">
         <v>116.4121952</v>
@@ -5079,11 +4933,10 @@
       <c r="J140" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" s="2" t="n">
-        <v>45696</v>
+        <v>45697</v>
       </c>
       <c r="B141" t="n">
         <v>116.4121952</v>
@@ -5112,11 +4965,10 @@
       <c r="J141" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" s="2" t="n">
-        <v>45697</v>
+        <v>45698</v>
       </c>
       <c r="B142" t="n">
         <v>116.4121952</v>
@@ -5145,11 +4997,10 @@
       <c r="J142" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" s="2" t="n">
-        <v>45698</v>
+        <v>45699</v>
       </c>
       <c r="B143" t="n">
         <v>116.4121952</v>
@@ -5178,11 +5029,10 @@
       <c r="J143" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" s="2" t="n">
-        <v>45699</v>
+        <v>45700</v>
       </c>
       <c r="B144" t="n">
         <v>116.4121952</v>
@@ -5211,11 +5061,10 @@
       <c r="J144" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" s="2" t="n">
-        <v>45700</v>
+        <v>45701</v>
       </c>
       <c r="B145" t="n">
         <v>116.4121952</v>
@@ -5244,11 +5093,10 @@
       <c r="J145" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" s="2" t="n">
-        <v>45701</v>
+        <v>45702</v>
       </c>
       <c r="B146" t="n">
         <v>116.4121952</v>
@@ -5277,11 +5125,10 @@
       <c r="J146" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" s="2" t="n">
-        <v>45702</v>
+        <v>45703</v>
       </c>
       <c r="B147" t="n">
         <v>116.4121952</v>
@@ -5310,11 +5157,10 @@
       <c r="J147" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" s="2" t="n">
-        <v>45703</v>
+        <v>45704</v>
       </c>
       <c r="B148" t="n">
         <v>116.4121952</v>
@@ -5343,11 +5189,10 @@
       <c r="J148" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" s="2" t="n">
-        <v>45704</v>
+        <v>45705</v>
       </c>
       <c r="B149" t="n">
         <v>116.4121952</v>
@@ -5376,11 +5221,10 @@
       <c r="J149" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" s="2" t="n">
-        <v>45705</v>
+        <v>45706</v>
       </c>
       <c r="B150" t="n">
         <v>116.4121952</v>
@@ -5409,11 +5253,10 @@
       <c r="J150" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" s="2" t="n">
-        <v>45706</v>
+        <v>45707</v>
       </c>
       <c r="B151" t="n">
         <v>116.4121952</v>
@@ -5442,11 +5285,10 @@
       <c r="J151" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" s="2" t="n">
-        <v>45707</v>
+        <v>45708</v>
       </c>
       <c r="B152" t="n">
         <v>116.4121952</v>
@@ -5475,11 +5317,10 @@
       <c r="J152" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K152" t="inlineStr"/>
     </row>
     <row r="153">
       <c r="A153" s="2" t="n">
-        <v>45708</v>
+        <v>45709</v>
       </c>
       <c r="B153" t="n">
         <v>116.4121952</v>
@@ -5508,11 +5349,10 @@
       <c r="J153" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K153" t="inlineStr"/>
     </row>
     <row r="154">
       <c r="A154" s="2" t="n">
-        <v>45709</v>
+        <v>45710</v>
       </c>
       <c r="B154" t="n">
         <v>116.4121952</v>
@@ -5541,11 +5381,10 @@
       <c r="J154" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K154" t="inlineStr"/>
     </row>
     <row r="155">
       <c r="A155" s="2" t="n">
-        <v>45710</v>
+        <v>45711</v>
       </c>
       <c r="B155" t="n">
         <v>116.4121952</v>
@@ -5574,11 +5413,10 @@
       <c r="J155" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" s="2" t="n">
-        <v>45711</v>
+        <v>45712</v>
       </c>
       <c r="B156" t="n">
         <v>116.4121952</v>
@@ -5607,11 +5445,10 @@
       <c r="J156" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K156" t="inlineStr"/>
     </row>
     <row r="157">
       <c r="A157" s="2" t="n">
-        <v>45712</v>
+        <v>45713</v>
       </c>
       <c r="B157" t="n">
         <v>116.4121952</v>
@@ -5640,11 +5477,10 @@
       <c r="J157" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" s="2" t="n">
-        <v>45713</v>
+        <v>45714</v>
       </c>
       <c r="B158" t="n">
         <v>116.4121952</v>
@@ -5673,11 +5509,10 @@
       <c r="J158" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K158" t="inlineStr"/>
     </row>
     <row r="159">
       <c r="A159" s="2" t="n">
-        <v>45714</v>
+        <v>45715</v>
       </c>
       <c r="B159" t="n">
         <v>116.4121952</v>
@@ -5706,11 +5541,10 @@
       <c r="J159" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K159" t="inlineStr"/>
     </row>
     <row r="160">
       <c r="A160" s="2" t="n">
-        <v>45715</v>
+        <v>45716</v>
       </c>
       <c r="B160" t="n">
         <v>116.4121952</v>
@@ -5739,11 +5573,10 @@
       <c r="J160" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" s="2" t="n">
-        <v>45716</v>
+        <v>45717</v>
       </c>
       <c r="B161" t="n">
         <v>116.4121952</v>
@@ -5772,11 +5605,10 @@
       <c r="J161" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K161" t="inlineStr"/>
     </row>
     <row r="162">
       <c r="A162" s="2" t="n">
-        <v>45717</v>
+        <v>45718</v>
       </c>
       <c r="B162" t="n">
         <v>116.4121952</v>
@@ -5805,11 +5637,10 @@
       <c r="J162" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K162" t="inlineStr"/>
     </row>
     <row r="163">
       <c r="A163" s="2" t="n">
-        <v>45718</v>
+        <v>45719</v>
       </c>
       <c r="B163" t="n">
         <v>116.4121952</v>
@@ -5838,11 +5669,10 @@
       <c r="J163" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K163" t="inlineStr"/>
     </row>
     <row r="164">
       <c r="A164" s="2" t="n">
-        <v>45719</v>
+        <v>45720</v>
       </c>
       <c r="B164" t="n">
         <v>116.4121952</v>
@@ -5871,11 +5701,10 @@
       <c r="J164" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K164" t="inlineStr"/>
     </row>
     <row r="165">
       <c r="A165" s="2" t="n">
-        <v>45720</v>
+        <v>45721</v>
       </c>
       <c r="B165" t="n">
         <v>116.4121952</v>
@@ -5904,11 +5733,10 @@
       <c r="J165" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K165" t="inlineStr"/>
     </row>
     <row r="166">
       <c r="A166" s="2" t="n">
-        <v>45721</v>
+        <v>45722</v>
       </c>
       <c r="B166" t="n">
         <v>116.4121952</v>
@@ -5937,11 +5765,10 @@
       <c r="J166" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K166" t="inlineStr"/>
     </row>
     <row r="167">
       <c r="A167" s="2" t="n">
-        <v>45722</v>
+        <v>45723</v>
       </c>
       <c r="B167" t="n">
         <v>116.4121952</v>
@@ -5970,11 +5797,10 @@
       <c r="J167" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K167" t="inlineStr"/>
     </row>
     <row r="168">
       <c r="A168" s="2" t="n">
-        <v>45723</v>
+        <v>45724</v>
       </c>
       <c r="B168" t="n">
         <v>116.4121952</v>
@@ -6003,11 +5829,10 @@
       <c r="J168" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K168" t="inlineStr"/>
     </row>
     <row r="169">
       <c r="A169" s="2" t="n">
-        <v>45724</v>
+        <v>45725</v>
       </c>
       <c r="B169" t="n">
         <v>116.4121952</v>
@@ -6036,11 +5861,10 @@
       <c r="J169" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" s="2" t="n">
-        <v>45725</v>
+        <v>45726</v>
       </c>
       <c r="B170" t="n">
         <v>116.4121952</v>
@@ -6069,11 +5893,10 @@
       <c r="J170" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K170" t="inlineStr"/>
     </row>
     <row r="171">
       <c r="A171" s="2" t="n">
-        <v>45726</v>
+        <v>45727</v>
       </c>
       <c r="B171" t="n">
         <v>116.4121952</v>
@@ -6102,11 +5925,10 @@
       <c r="J171" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K171" t="inlineStr"/>
     </row>
     <row r="172">
       <c r="A172" s="2" t="n">
-        <v>45727</v>
+        <v>45728</v>
       </c>
       <c r="B172" t="n">
         <v>116.4121952</v>
@@ -6135,11 +5957,10 @@
       <c r="J172" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K172" t="inlineStr"/>
     </row>
     <row r="173">
       <c r="A173" s="2" t="n">
-        <v>45728</v>
+        <v>45729</v>
       </c>
       <c r="B173" t="n">
         <v>116.4121952</v>
@@ -6168,11 +5989,10 @@
       <c r="J173" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K173" t="inlineStr"/>
     </row>
     <row r="174">
       <c r="A174" s="2" t="n">
-        <v>45729</v>
+        <v>45730</v>
       </c>
       <c r="B174" t="n">
         <v>116.4121952</v>
@@ -6201,11 +6021,10 @@
       <c r="J174" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K174" t="inlineStr"/>
     </row>
     <row r="175">
       <c r="A175" s="2" t="n">
-        <v>45730</v>
+        <v>45731</v>
       </c>
       <c r="B175" t="n">
         <v>116.4121952</v>
@@ -6234,11 +6053,10 @@
       <c r="J175" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K175" t="inlineStr"/>
     </row>
     <row r="176">
       <c r="A176" s="2" t="n">
-        <v>45731</v>
+        <v>45732</v>
       </c>
       <c r="B176" t="n">
         <v>116.4121952</v>
@@ -6267,11 +6085,10 @@
       <c r="J176" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K176" t="inlineStr"/>
     </row>
     <row r="177">
       <c r="A177" s="2" t="n">
-        <v>45732</v>
+        <v>45733</v>
       </c>
       <c r="B177" t="n">
         <v>116.4121952</v>
@@ -6300,40 +6117,6 @@
       <c r="J177" t="n">
         <v>485.38834923</v>
       </c>
-      <c r="K177" t="inlineStr"/>
-    </row>
-    <row r="178">
-      <c r="A178" s="2" t="n">
-        <v>45733</v>
-      </c>
-      <c r="B178" t="n">
-        <v>116.4121952</v>
-      </c>
-      <c r="C178" t="n">
-        <v>0.00170247</v>
-      </c>
-      <c r="D178" t="n">
-        <v>0.008850780000000001</v>
-      </c>
-      <c r="E178" t="n">
-        <v>0.06933635</v>
-      </c>
-      <c r="F178" t="n">
-        <v>12792.90181321</v>
-      </c>
-      <c r="G178" t="n">
-        <v>465.80531254</v>
-      </c>
-      <c r="H178" t="n">
-        <v>0.24</v>
-      </c>
-      <c r="I178" t="n">
-        <v>1.7904431</v>
-      </c>
-      <c r="J178" t="n">
-        <v>485.38834923</v>
-      </c>
-      <c r="K178" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>